<commit_message>
Updated design fabrication files
</commit_message>
<xml_diff>
--- a/test-hardware/hardware-design/Power-Control-V1-Layer/20230827-JLCPCB-Unplaced-Components.xlsx
+++ b/test-hardware/hardware-design/Power-Control-V1-Layer/20230827-JLCPCB-Unplaced-Components.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parke\Documents\GitHub\Electrical_mCLARI\test-hardware\hardware-design\Power-Control-V1-Layer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5F7B93F-995D-4311-B527-D4DAF680F5FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D5230C1-543C-4398-BD61-CAFCFBE99153}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -542,7 +542,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="A24:C24"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>